<commit_message>
had a bug, fixed it
</commit_message>
<xml_diff>
--- a/Fatture.xlsx
+++ b/Fatture.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J350"/>
+  <dimension ref="A1:J374"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11069,7 +11069,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H323" t="inlineStr"/>
       <c r="I323" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -11107,7 +11106,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H324" t="inlineStr"/>
       <c r="I324" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -11145,7 +11143,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H325" t="inlineStr"/>
       <c r="I325" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -11183,7 +11180,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H326" t="inlineStr"/>
       <c r="I326" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -11221,7 +11217,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H327" t="inlineStr"/>
       <c r="I327" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -11259,7 +11254,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H328" t="inlineStr"/>
       <c r="I328" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -11297,7 +11291,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H329" t="inlineStr"/>
       <c r="I329" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -11335,7 +11328,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H330" t="inlineStr"/>
       <c r="I330" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -11373,7 +11365,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H331" t="inlineStr"/>
       <c r="I331" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -11411,7 +11402,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H332" t="inlineStr"/>
       <c r="I332" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -11449,7 +11439,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H333" t="inlineStr"/>
       <c r="I333" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -11487,7 +11476,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H334" t="inlineStr"/>
       <c r="I334" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -12126,6 +12114,496 @@
       <c r="J350" t="inlineStr">
         <is>
           <t>70,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ADRIATICA	LUCIDANTI	DI	PETRIZZO
+GIANLUCA	C	SNC
+</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>31-03-2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>LUCIDANTE	POTE	GRANITO</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="F354" t="inlineStr">
+        <is>
+          <t>13,60</t>
+        </is>
+      </c>
+      <c r="G354" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="I354" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J354" t="inlineStr">
+        <is>
+          <t>68,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>CASSANI	SUPER	GR	30/60/120</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>135,00</t>
+        </is>
+      </c>
+      <c r="F355" t="inlineStr">
+        <is>
+          <t>0,97</t>
+        </is>
+      </c>
+      <c r="G355" t="inlineStr">
+        <is>
+          <t>PZ</t>
+        </is>
+      </c>
+      <c r="I355" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J355" t="inlineStr">
+        <is>
+          <t>130,95</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>LUCIDANTE	F1</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>50,00</t>
+        </is>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>4,30</t>
+        </is>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="I356" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J356" t="inlineStr">
+        <is>
+          <t>215,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>LUCIDANTE	WR	MARMO</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>50,00</t>
+        </is>
+      </c>
+      <c r="F357" t="inlineStr">
+        <is>
+          <t>4,60</t>
+        </is>
+      </c>
+      <c r="G357" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="I357" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J357" t="inlineStr">
+        <is>
+          <t>230,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NP	DIAMANT	SRLS
+</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>27-02-2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>DISCO	D.350	B2DLC/2	SILENZIATO	GRANITO	F.50</t>
+        </is>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="F361" t="inlineStr">
+        <is>
+          <t>51,00</t>
+        </is>
+      </c>
+      <c r="G361" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I361" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J361" t="inlineStr">
+        <is>
+          <t>51,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>DISCO	D.400	B2DLC/2	SILENZIATO	GRANITO</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="F362" t="inlineStr">
+        <is>
+          <t>67,00</t>
+        </is>
+      </c>
+      <c r="G362" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I362" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J362" t="inlineStr">
+        <is>
+          <t>134,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>DISCO	D.500	B2DLC/2	SILENZIATO	GRANITO</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>106,00</t>
+        </is>
+      </c>
+      <c r="G363" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I363" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J363" t="inlineStr">
+        <is>
+          <t>106,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>DISCO	D.500	M1S	SILENZIATO	MARMO	F.60/50</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>112,00</t>
+        </is>
+      </c>
+      <c r="G364" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I364" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J364" t="inlineStr">
+        <is>
+          <t>112,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>DISCO	D.625	V55DLC/2	SILENZIATO	PER</t>
+        </is>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="F365" t="inlineStr">
+        <is>
+          <t>245,10</t>
+        </is>
+      </c>
+      <c r="G365" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I365" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J365" t="inlineStr">
+        <is>
+          <t>245,10</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>FRESA	DA	TAGLIO	22*45	ATT.1/2	GAS	5	SETTORI</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="F366" t="inlineStr">
+        <is>
+          <t>50,00</t>
+        </is>
+      </c>
+      <c r="G366" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I366" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J366" t="inlineStr">
+        <is>
+          <t>100,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>DISCO	D.230	D.E.	F.25,4	MARMO</t>
+        </is>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="F367" t="inlineStr">
+        <is>
+          <t>28,00</t>
+        </is>
+      </c>
+      <c r="G367" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I367" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J367" t="inlineStr">
+        <is>
+          <t>28,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>MOLA	D.240X437	RIGENERATA	CONH	220</t>
+        </is>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="F368" t="inlineStr">
+        <is>
+          <t>619,00</t>
+        </is>
+      </c>
+      <c r="G368" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I368" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J368" t="inlineStr">
+        <is>
+          <t>619,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SWEDIAM	SRL
+</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>29-01-2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SWEDIAM	SRL
+</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>29-01-2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SWEDIAM	SRL
+</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>26-02-2021</t>
         </is>
       </c>
     </row>
@@ -12196,7 +12674,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C1:L349"/>
+  <dimension ref="C1:L367"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22678,7 +23156,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H322" t="inlineStr"/>
       <c r="I322" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -22716,7 +23193,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H323" t="inlineStr"/>
       <c r="I323" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -22754,7 +23230,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H324" t="inlineStr"/>
       <c r="I324" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -22792,7 +23267,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H325" t="inlineStr"/>
       <c r="I325" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -22830,7 +23304,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H326" t="inlineStr"/>
       <c r="I326" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -22868,7 +23341,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H327" t="inlineStr"/>
       <c r="I327" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -22906,7 +23378,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H328" t="inlineStr"/>
       <c r="I328" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -22944,7 +23415,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H329" t="inlineStr"/>
       <c r="I329" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -22982,7 +23452,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H330" t="inlineStr"/>
       <c r="I330" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -23020,7 +23489,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H331" t="inlineStr"/>
       <c r="I331" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -23058,7 +23526,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H332" t="inlineStr"/>
       <c r="I332" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -23096,7 +23563,6 @@
           <t>NR</t>
         </is>
       </c>
-      <c r="H333" t="inlineStr"/>
       <c r="I333" t="inlineStr">
         <is>
           <t>22,00</t>
@@ -23735,6 +24201,430 @@
       <c r="J349" t="inlineStr">
         <is>
           <t>70,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>LUCIDANTE	POTE	GRANITO</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>5,00</t>
+        </is>
+      </c>
+      <c r="F353" t="inlineStr">
+        <is>
+          <t>13,60</t>
+        </is>
+      </c>
+      <c r="G353" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="I353" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J353" t="inlineStr">
+        <is>
+          <t>68,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>CASSANI	SUPER	GR	30/60/120</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>135,00</t>
+        </is>
+      </c>
+      <c r="F354" t="inlineStr">
+        <is>
+          <t>0,97</t>
+        </is>
+      </c>
+      <c r="G354" t="inlineStr">
+        <is>
+          <t>PZ</t>
+        </is>
+      </c>
+      <c r="I354" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J354" t="inlineStr">
+        <is>
+          <t>130,95</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>LUCIDANTE	F1</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>50,00</t>
+        </is>
+      </c>
+      <c r="F355" t="inlineStr">
+        <is>
+          <t>4,30</t>
+        </is>
+      </c>
+      <c r="G355" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="I355" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J355" t="inlineStr">
+        <is>
+          <t>215,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>LUCIDANTE	WR	MARMO</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>50,00</t>
+        </is>
+      </c>
+      <c r="F356" t="inlineStr">
+        <is>
+          <t>4,60</t>
+        </is>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="I356" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J356" t="inlineStr">
+        <is>
+          <t>230,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>DISCO	D.350	B2DLC/2	SILENZIATO	GRANITO	F.50</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="F360" t="inlineStr">
+        <is>
+          <t>51,00</t>
+        </is>
+      </c>
+      <c r="G360" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I360" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J360" t="inlineStr">
+        <is>
+          <t>51,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>DISCO	D.400	B2DLC/2	SILENZIATO	GRANITO</t>
+        </is>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="F361" t="inlineStr">
+        <is>
+          <t>67,00</t>
+        </is>
+      </c>
+      <c r="G361" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I361" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J361" t="inlineStr">
+        <is>
+          <t>134,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>DISCO	D.500	B2DLC/2	SILENZIATO	GRANITO</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="F362" t="inlineStr">
+        <is>
+          <t>106,00</t>
+        </is>
+      </c>
+      <c r="G362" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I362" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J362" t="inlineStr">
+        <is>
+          <t>106,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>DISCO	D.500	M1S	SILENZIATO	MARMO	F.60/50</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="F363" t="inlineStr">
+        <is>
+          <t>112,00</t>
+        </is>
+      </c>
+      <c r="G363" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I363" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J363" t="inlineStr">
+        <is>
+          <t>112,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>DISCO	D.625	V55DLC/2	SILENZIATO	PER</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="F364" t="inlineStr">
+        <is>
+          <t>245,10</t>
+        </is>
+      </c>
+      <c r="G364" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I364" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J364" t="inlineStr">
+        <is>
+          <t>245,10</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>FRESA	DA	TAGLIO	22*45	ATT.1/2	GAS	5	SETTORI</t>
+        </is>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>2,00</t>
+        </is>
+      </c>
+      <c r="F365" t="inlineStr">
+        <is>
+          <t>50,00</t>
+        </is>
+      </c>
+      <c r="G365" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I365" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J365" t="inlineStr">
+        <is>
+          <t>100,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>DISCO	D.230	D.E.	F.25,4	MARMO</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="F366" t="inlineStr">
+        <is>
+          <t>28,00</t>
+        </is>
+      </c>
+      <c r="G366" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I366" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J366" t="inlineStr">
+        <is>
+          <t>28,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>MOLA	D.240X437	RIGENERATA	CONH	220</t>
+        </is>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+      <c r="F367" t="inlineStr">
+        <is>
+          <t>619,00</t>
+        </is>
+      </c>
+      <c r="G367" t="inlineStr">
+        <is>
+          <t>NR</t>
+        </is>
+      </c>
+      <c r="I367" t="inlineStr">
+        <is>
+          <t>22,00</t>
+        </is>
+      </c>
+      <c r="J367" t="inlineStr">
+        <is>
+          <t>619,00</t>
         </is>
       </c>
     </row>

</xml_diff>